<commit_message>
adding area to dishcarge files
</commit_message>
<xml_diff>
--- a/Discharge/Station1_2021-06-09_1127.xlsx
+++ b/Discharge/Station1_2021-06-09_1127.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/kriddie_ad_unc_edu/Documents/Ecuador2021/Ecuador2021/Discharge/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1cba20500feb7d90/Documents/LongTermData_CayambeCoca/Discharge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_A416E8928F630E045B335349C9CA984D21398A2A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55F9A91C-83D8-104F-95EA-C67C9901AF65}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_A416E8928F630E045B335349C9CA984D21398A2A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C7250BB-C8CE-4A2D-9577-50BA28B2597F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1070" windowWidth="8720" windowHeight="9730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>x</t>
   </si>
@@ -53,6 +52,12 @@
   </si>
   <si>
     <t>Qtotal</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Atotal</t>
   </si>
 </sst>
 </file>
@@ -370,15 +375,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="G1" sqref="G1:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -397,8 +402,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>60</v>
       </c>
@@ -416,8 +427,16 @@
         <f>SUM(E2:E20)</f>
         <v>4.4454999999999998E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <f>(D2-0)*B2/100</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>SUM(G2:G11)</f>
+        <v>7.4049999999999991E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>63</v>
       </c>
@@ -435,8 +454,12 @@
         <f t="shared" ref="E3:E19" si="0">(D3-D2)*(B3/100)*C3</f>
         <v>7.1500000000000057E-5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <f>(D3-D2)*B3/100</f>
+        <v>7.1500000000000062E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>70</v>
       </c>
@@ -454,8 +477,12 @@
         <f>(D4-D3)*(B4/100)*C4</f>
         <v>8.3999999999999928E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <f t="shared" ref="G4:G11" si="1">(D4-D3)*B4/100</f>
+        <v>8.3999999999999925E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>75</v>
       </c>
@@ -473,8 +500,12 @@
         <f>(D5-D4)*(B5/100)*C5</f>
         <v>2.7000000000000022E-4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>9.000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>80</v>
       </c>
@@ -485,15 +516,19 @@
         <v>0.09</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D19" si="1">(A6/100+(A7/100-A6/100)/2)</f>
+        <f t="shared" ref="D6:D19" si="2">(A6/100+(A7/100-A6/100)/2)</f>
         <v>0.82499999999999996</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
         <v>9.4499999999999858E-4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>1.0499999999999985E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>85</v>
       </c>
@@ -504,15 +539,19 @@
         <v>0.15</v>
       </c>
       <c r="D7">
+        <f t="shared" si="2"/>
+        <v>0.875</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1.7250000000000015E-3</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="1"/>
-        <v>0.875</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>1.7250000000000015E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.150000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>90</v>
       </c>
@@ -523,15 +562,19 @@
         <v>0.06</v>
       </c>
       <c r="D8">
+        <f t="shared" si="2"/>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>7.5000000000000067E-4</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="1"/>
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>7.5000000000000067E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.2500000000000011E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>95</v>
       </c>
@@ -542,15 +585,19 @@
         <v>0.04</v>
       </c>
       <c r="D9">
+        <f t="shared" si="2"/>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999919E-4</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="1"/>
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>5.9999999999999919E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>100</v>
       </c>
@@ -561,27 +608,35 @@
         <v>0</v>
       </c>
       <c r="D10">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E12">
@@ -589,9 +644,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E13">
@@ -599,9 +654,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E14">
@@ -609,9 +664,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E15">
@@ -619,9 +674,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E16">
@@ -629,9 +684,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E17">
@@ -639,9 +694,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E18">
@@ -649,9 +704,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E19">

</xml_diff>